<commit_message>
Fiexed Bug with index column
</commit_message>
<xml_diff>
--- a/excel_report.xlsx
+++ b/excel_report.xlsx
@@ -488,17 +488,17 @@
           <t>SCPI Version</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Gain</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Gain</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Offset</t>
         </is>
@@ -514,18 +514,15 @@
       <c r="B2" t="n">
         <v>1995</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Voltage</t>
         </is>
       </c>
+      <c r="G2" t="n">
+        <v>0.00025</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.00025</v>
-      </c>
-      <c r="I2" t="n">
         <v>0.0015</v>
       </c>
     </row>
@@ -559,7 +556,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2023-07-06 16:13:06</t>
+          <t>2023-07-07 08:58:55</t>
         </is>
       </c>
     </row>
@@ -636,16 +633,16 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.499698929</v>
+        <v>0.499869907</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0003010709999999</v>
+        <v>0.0001300929999999</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0602141999999972</v>
+        <v>0.0260185999999995</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -674,16 +671,16 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>1.49871027</v>
+        <v>1.49904498</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0012897300000001</v>
+        <v>0.0009550199999999</v>
       </c>
       <c r="H10" t="n">
-        <v>0.08598200000000659</v>
+        <v>0.06366799999999451</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -712,16 +709,16 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>2.49838673</v>
+        <v>2.49806191</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00161327</v>
+        <v>0.0019380899999998</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0645308</v>
+        <v>0.0775235999999957</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -750,16 +747,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>3.49877894</v>
+        <v>3.49804021</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0012210600000002</v>
+        <v>0.0019597899999999</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0348874285714348</v>
+        <v>0.0559939999999973</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -788,16 +785,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>4.4986207</v>
+        <v>4.49849235</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0013792999999999</v>
+        <v>0.0015076499999997</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0306511111111104</v>
+        <v>0.0335033333333277</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -826,16 +823,16 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>5.49873932</v>
+        <v>5.49847591</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0012606799999996</v>
+        <v>0.0015240900000002</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0229214545454487</v>
+        <v>0.0277107272727309</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -864,16 +861,16 @@
         <v>2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.499347486</v>
+        <v>0.499244162</v>
       </c>
       <c r="F15" t="n">
         <v>2</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0006525139999999</v>
+        <v>0.000755838</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1305027999999986</v>
+        <v>0.1511676000000017</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -888,7 +885,7 @@
         <v>-0.1501249999999999</v>
       </c>
       <c r="M15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -902,16 +899,16 @@
         <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>1.49861593</v>
+        <v>1.49819604</v>
       </c>
       <c r="F16" t="n">
         <v>2</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00138407</v>
+        <v>0.0018039599999999</v>
       </c>
       <c r="H16" t="n">
-        <v>0.09227133333333799</v>
+        <v>0.1202639999999958</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -940,16 +937,16 @@
         <v>2</v>
       </c>
       <c r="E17" t="n">
-        <v>2.498049</v>
+        <v>2.49810439</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>0.001951</v>
+        <v>0.00189561</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0780400000000014</v>
+        <v>0.0758244000000019</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -978,16 +975,16 @@
         <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>3.498242</v>
+        <v>3.49757251</v>
       </c>
       <c r="F18" t="n">
         <v>2</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0017580000000001</v>
+        <v>0.00242749</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0502285714285756</v>
+        <v>0.06935685714285959</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1016,16 +1013,16 @@
         <v>2</v>
       </c>
       <c r="E19" t="n">
-        <v>4.49799744</v>
+        <v>4.4977456</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0020025600000002</v>
+        <v>0.0022543999999999</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0445013333333379</v>
+        <v>0.0500977777777775</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1054,16 +1051,16 @@
         <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>5.49830401</v>
+        <v>5.4982261</v>
       </c>
       <c r="F20" t="n">
         <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0016959899999999</v>
+        <v>0.0017738999999998</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0308361818181814</v>
+        <v>0.0322527272727251</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>

</xml_diff>